<commit_message>
Newe Item Page started
</commit_message>
<xml_diff>
--- a/data/types.xlsx
+++ b/data/types.xlsx
@@ -11,13 +11,14 @@
     <sheet name="ΠΑΡΑΘΥΡΑ" sheetId="2" r:id="rId2"/>
     <sheet name="ΣΕΙΡΩΜΕΝΑ" sheetId="3" r:id="rId3"/>
     <sheet name="ΚΕΝΤΡΙΚΕΣ ΕΙΣΟΔΟΙ" sheetId="4" r:id="rId4"/>
+    <sheet name="TEST" sheetId="7" r:id="rId5"/>
   </sheets>
   <calcPr calcId="144525"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="236" uniqueCount="126">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="249" uniqueCount="128">
   <si>
     <t>ΤΥΠΟΙ</t>
   </si>
@@ -397,6 +398,12 @@
   </si>
   <si>
     <t>Ελάχιστο Ύψος</t>
+  </si>
+  <si>
+    <t>TEST 6-φυλλο</t>
+  </si>
+  <si>
+    <t>TEST-6-SLD</t>
   </si>
 </sst>
 </file>
@@ -2915,12 +2922,12 @@
   <dimension ref="A1:K20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B24" sqref="B24"/>
+      <selection activeCell="G24" sqref="G24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="29.42578125" style="24" customWidth="1"/>
+    <col min="1" max="1" width="48.85546875" style="24" customWidth="1"/>
     <col min="2" max="2" width="22.140625" style="24" customWidth="1"/>
     <col min="3" max="3" width="9.140625" style="24"/>
     <col min="4" max="4" width="10.42578125" style="24" customWidth="1"/>
@@ -3059,7 +3066,7 @@
         <v>1</v>
       </c>
       <c r="D5" s="13">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E5" s="14">
         <v>0</v>
@@ -3164,7 +3171,7 @@
         <v>4</v>
       </c>
       <c r="D8" s="13">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E8" s="14">
         <v>1</v>
@@ -3199,7 +3206,7 @@
         <v>11</v>
       </c>
       <c r="D9" s="13">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E9" s="14">
         <v>0</v>
@@ -3234,7 +3241,7 @@
         <v>11</v>
       </c>
       <c r="D10" s="13">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E10" s="14">
         <v>0</v>
@@ -3269,7 +3276,7 @@
         <v>11</v>
       </c>
       <c r="D11" s="13">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="E11" s="14">
         <v>0</v>
@@ -3374,7 +3381,7 @@
         <v>12</v>
       </c>
       <c r="D14" s="13">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="E14" s="14">
         <v>0</v>
@@ -3409,7 +3416,7 @@
         <v>13</v>
       </c>
       <c r="D15" s="13">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="E15" s="14">
         <v>0</v>
@@ -3444,7 +3451,7 @@
         <v>13</v>
       </c>
       <c r="D16" s="13">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E16" s="14">
         <v>0</v>
@@ -3479,7 +3486,7 @@
         <v>13</v>
       </c>
       <c r="D17" s="13">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="E17" s="14">
         <v>0</v>
@@ -3511,7 +3518,7 @@
         <v>14</v>
       </c>
       <c r="D18" s="13">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E18" s="14">
         <v>1</v>
@@ -3543,7 +3550,7 @@
         <v>14</v>
       </c>
       <c r="D19" s="13">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E19" s="14">
         <v>1</v>
@@ -3575,7 +3582,7 @@
         <v>14</v>
       </c>
       <c r="D20" s="13">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="E20" s="14">
         <v>1</v>
@@ -3595,6 +3602,117 @@
       <c r="J20" s="15">
         <v>0</v>
       </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:L3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="29.42578125" customWidth="1"/>
+    <col min="2" max="2" width="32" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+      <c r="A1" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="23" t="s">
+        <v>37</v>
+      </c>
+      <c r="C1" s="16" t="s">
+        <v>82</v>
+      </c>
+      <c r="D1" s="20" t="s">
+        <v>115</v>
+      </c>
+      <c r="E1" s="21" t="s">
+        <v>116</v>
+      </c>
+      <c r="F1" s="22" t="s">
+        <v>117</v>
+      </c>
+      <c r="G1" s="18" t="s">
+        <v>123</v>
+      </c>
+      <c r="H1" s="19" t="s">
+        <v>122</v>
+      </c>
+      <c r="I1" s="18" t="s">
+        <v>124</v>
+      </c>
+      <c r="J1" s="19" t="s">
+        <v>125</v>
+      </c>
+      <c r="K1" s="24"/>
+      <c r="L1" s="24"/>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A2" s="3"/>
+      <c r="B2" s="24"/>
+      <c r="C2" s="17"/>
+      <c r="D2" s="13"/>
+      <c r="E2" s="14"/>
+      <c r="F2" s="15"/>
+      <c r="G2" s="14">
+        <v>0</v>
+      </c>
+      <c r="H2" s="15">
+        <v>0</v>
+      </c>
+      <c r="I2" s="14">
+        <v>0</v>
+      </c>
+      <c r="J2" s="15">
+        <v>0</v>
+      </c>
+      <c r="K2" s="24"/>
+      <c r="L2" s="24"/>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A3" s="28" t="s">
+        <v>126</v>
+      </c>
+      <c r="B3" s="31" t="s">
+        <v>127</v>
+      </c>
+      <c r="C3" s="17">
+        <v>1</v>
+      </c>
+      <c r="D3" s="13">
+        <v>6</v>
+      </c>
+      <c r="E3" s="14">
+        <v>0</v>
+      </c>
+      <c r="F3" s="15">
+        <v>0</v>
+      </c>
+      <c r="G3" s="14">
+        <v>0</v>
+      </c>
+      <c r="H3" s="15">
+        <v>0</v>
+      </c>
+      <c r="I3" s="14">
+        <v>0</v>
+      </c>
+      <c r="J3" s="15">
+        <v>0</v>
+      </c>
+      <c r="K3" s="24" t="s">
+        <v>83</v>
+      </c>
+      <c r="L3" s="24"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>